<commit_message>
Adjustments to DSGE class
</commit_message>
<xml_diff>
--- a/Utilities/prior_table.xlsx
+++ b/Utilities/prior_table.xlsx
@@ -1,31 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamarante\PycharmProjects\pygensys\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoamarante/PycharmProjects/pydsge/Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617B8A05-4476-41AE-832D-CCD8ED89F1D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3666AFA0-2D10-E541-A657-7E34F3079B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19440" windowHeight="15160" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Iterações" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -171,7 +165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,16 +463,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ADE82D-4C65-4E41-9CFD-12B21879D657}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -495,7 +489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +512,7 @@
         <v>8.298826628866153E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -541,7 +535,7 @@
         <v>1.2247448713915889</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -565,7 +559,7 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +582,7 @@
         <v>0.28867513459481287</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,7 +605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -622,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -636,7 +630,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -650,7 +644,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -664,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -678,7 +672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -692,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -706,7 +700,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -720,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -734,7 +728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -748,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -762,7 +756,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -779,32 +773,31 @@
   <dimension ref="C1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1">
-        <f>6+7</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2">
-        <v>2.15</v>
+        <v>2.1</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <f>C1*3600*C2</f>
-        <v>100620</v>
+        <v>151200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prior inputs are now mean and std
</commit_message>
<xml_diff>
--- a/Utilities/prior_table.xlsx
+++ b/Utilities/prior_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamarante\PycharmProjects\pydsge\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoamarante/PycharmProjects/pydsge/Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C14F319-0BC5-46AA-ACB6-66D115586167}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5978DF-FC4E-9944-AE91-9A384552BA3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="1" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22820" windowHeight="17440" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -45,23 +45,17 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Beta</t>
   </si>
@@ -123,16 +117,16 @@
     <t>sigma_v</t>
   </si>
   <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>obj</t>
-  </si>
-  <si>
     <t>theta</t>
   </si>
   <si>
     <t>sigma_pi</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -212,7 +206,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -508,18 +502,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ADE82D-4C65-4E41-9CFD-12B21879D657}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
@@ -535,50 +529,45 @@
       <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>2.9999998688322576</v>
+        <v>1.5</v>
       </c>
       <c r="C2" s="4">
-        <v>1.9999999450453154</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="3">
         <f>B2/(B2+C2)</f>
-        <v>0.59999999610114263</v>
+        <v>0.5</v>
       </c>
       <c r="E2" s="3">
         <f>(B2*C2)/(((B2+C2)^2)*(B2+C2+1))</f>
-        <v>4.0000001370778131E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F2" s="3">
         <f>SQRT(E2)</f>
-        <v>0.20000000342694529</v>
+        <v>0.25</v>
       </c>
       <c r="H2">
-        <v>0.6</v>
+        <f>((D2^2)*(1-D2))/E2-D2</f>
+        <v>1.5</v>
       </c>
       <c r="I2">
-        <v>0.2</v>
-      </c>
-      <c r="J2">
-        <f>100*((D2-H2)^2+(I2-F2)^2)</f>
-        <v>2.6945042594084682E-15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f>H2*(1-D2)/D2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -601,17 +590,15 @@
         <v>9.9599196783909855E-2</v>
       </c>
       <c r="H3">
-        <v>0.25</v>
+        <f>(D3/F3)^2</f>
+        <v>6.200000000000002</v>
       </c>
       <c r="I3">
-        <v>0.1</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J6" si="0">100*((D3-H3)^2+(I3-F3)^2)</f>
-        <v>4.1606432180281048E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <f>D3/H3</f>
+        <v>3.9999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -634,17 +621,15 @@
         <v>0.250000000005138</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <f>(D4/F4)^2+2</f>
+        <v>5.999999998917688</v>
       </c>
       <c r="I4">
-        <v>0.25</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>3.3175437148600886E-19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <f>D4*(H4-1)</f>
+        <v>2.4999999991720014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -667,17 +652,15 @@
         <v>0.28867513459481287</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <f>D5-SQRT(3)*F5</f>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.28867513459481287</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f>2*D5-H5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -700,17 +683,15 @@
         <v>3</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <f>D6</f>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>0.3</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <f>F6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
@@ -721,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -735,9 +716,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -749,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -763,7 +744,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -777,7 +758,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -791,7 +772,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -805,7 +786,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -819,7 +800,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -833,9 +814,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>2</v>
@@ -857,13 +838,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DF6D28-0B61-407D-A00A-C6152F94AC75}">
   <dimension ref="C1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1">
         <v>1.5</v>
       </c>
@@ -871,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2">
         <v>2.1</v>
       </c>
@@ -879,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3">
         <f>C1*3600*C2</f>
         <v>11340</v>
@@ -900,12 +881,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D294B0ABAE3DD40AEF644D986102746" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="afcae322f938b1831e997e755636afc1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="041f13eb0e079512118c42f2f99b7046" ns3:_="">
     <xsd:import namespace="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
@@ -1037,6 +1012,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE9D510-3DE7-4BF6-9275-165518CBD85E}">
   <ds:schemaRefs>
@@ -1046,22 +1027,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A1D3B3-1A39-4D4D-BFE6-D76A5FF26CFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB112CA5-772D-401E-B7BD-FCD9C5E40A48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1077,4 +1042,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A1D3B3-1A39-4D4D-BFE6-D76A5FF26CFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
minor changes to the DSGE class
</commit_message>
<xml_diff>
--- a/Utilities/prior_table.xlsx
+++ b/Utilities/prior_table.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamarante\PycharmProjects\pydsge_latest\Utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoamarante/PycharmProjects/pydsge/Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A856764B-7C64-444D-8D02-ACB17E63BA7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF6F41-B5A7-744D-8C89-7A25BF8076B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19440" windowHeight="15160" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Distribuições" sheetId="1" r:id="rId1"/>
-    <sheet name="Iterações" sheetId="2" r:id="rId2"/>
+    <sheet name="Priors" sheetId="1" r:id="rId1"/>
+    <sheet name="Iterations Calculator" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Distribuições!#REF!</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Priors!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -31,7 +31,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Distribuições!$F$2</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Priors!$F$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -45,23 +45,17 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Beta</t>
   </si>
@@ -78,48 +72,12 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>Param b</t>
-  </si>
-  <si>
-    <t>Param a</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
     <t>Std</t>
   </si>
   <si>
-    <t>Dist</t>
-  </si>
-  <si>
-    <t>sigma</t>
-  </si>
-  <si>
-    <t>phi_pi</t>
-  </si>
-  <si>
-    <t>phi_y</t>
-  </si>
-  <si>
-    <t>rho_a</t>
-  </si>
-  <si>
-    <t>sigma_a</t>
-  </si>
-  <si>
-    <t>rho_v</t>
-  </si>
-  <si>
-    <t>sigma_v</t>
-  </si>
-  <si>
-    <t>theta</t>
-  </si>
-  <si>
-    <t>sigma_pi</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -148,6 +106,18 @@
   </si>
   <si>
     <t>Iterations</t>
+  </si>
+  <si>
+    <t>I suggest running a simulation with a chain size of 2000 and see how long it takes.</t>
+  </si>
+  <si>
+    <t>Then you can set "End Time" as when you want the estimation process to stop.</t>
+  </si>
+  <si>
+    <t>The calculator will show you the approximate size of the MCMC chains you have to set.</t>
+  </si>
+  <si>
+    <t>For each distribution you can choose the mean and standard deviation. The calculator will give you the distribution parameters.</t>
   </si>
 </sst>
 </file>
@@ -179,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,20 +238,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -297,6 +286,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -317,7 +324,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -613,261 +620,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ADE82D-4C65-4E41-9CFD-12B21879D657}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B4" s="15">
         <v>0.5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C4" s="16">
         <v>0.2</v>
       </c>
-      <c r="D2">
-        <f>((B2^2)*(1-B2))/(C2^2)-B2</f>
+      <c r="D4" s="3">
+        <f>((B4^2)*(1-B4))/(C4^2)-B4</f>
         <v>2.6249999999999996</v>
       </c>
-      <c r="E2">
-        <f>D2*(1-B2)/B2</f>
+      <c r="E4" s="3">
+        <f>D4*(1-B4)/B4</f>
         <v>2.6249999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B5" s="17">
         <v>0.24800000000000003</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C5" s="18">
         <v>9.9599196783909855E-2</v>
       </c>
-      <c r="D3">
-        <f>(B3/C3)^2</f>
+      <c r="D5" s="3">
+        <f>(B5/C5)^2</f>
         <v>6.200000000000002</v>
       </c>
-      <c r="E3">
-        <f>B3/D3</f>
+      <c r="E5" s="3">
+        <f>B5/D5</f>
         <v>3.9999999999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B6" s="17">
         <v>0.4999999999426315</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C6" s="18">
         <v>0.250000000005138</v>
       </c>
-      <c r="D4">
-        <f>(B4/C4)^2+2</f>
+      <c r="D6" s="3">
+        <f>(B6/C6)^2+2</f>
         <v>5.999999998917688</v>
       </c>
-      <c r="E4">
-        <f>B4*(D4-1)</f>
+      <c r="E6" s="3">
+        <f>B6*(D6-1)</f>
         <v>2.4999999991720014</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B7" s="17">
         <v>0.5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C7" s="18">
         <v>0.28867513459481287</v>
       </c>
-      <c r="D5">
-        <f>B5-SQRT(3)*C5</f>
+      <c r="D7" s="3">
+        <f>B7-SQRT(3)*C7</f>
         <v>0</v>
       </c>
-      <c r="E5">
-        <f>2*B5-D5</f>
+      <c r="E7" s="3">
+        <f>2*B7-D7</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" s="20">
         <v>3</v>
       </c>
-      <c r="D6">
-        <f>B6</f>
+      <c r="D8" s="3">
+        <f>B8</f>
         <v>3</v>
       </c>
-      <c r="E6">
-        <f>C6</f>
+      <c r="E8" s="3">
+        <f>C8</f>
         <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3">
-        <v>6</v>
-      </c>
-      <c r="D15" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="3">
-        <v>6</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>6</v>
-      </c>
-      <c r="D18" s="3">
-        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -878,86 +754,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DF6D28-0B61-407D-A00A-C6152F94AC75}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
         <v>2000</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="13">
-        <v>43698.291666666664</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="12">
+        <v>44023.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="7">
         <v>48</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="12">
-        <f ca="1">(F4-NOW())*24*3600*B8</f>
-        <v>-41482.288136257463</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <f>B3/(B6+60*B5+3600*B4)</f>
+      <c r="C9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11">
+        <f ca="1">(F7-NOW())*24*3600*B11</f>
+        <v>183448.58757089984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4">
+        <f>B6/(B9+60*B8+3600*B7)</f>
         <v>2.8248587570621471</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -971,6 +862,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D294B0ABAE3DD40AEF644D986102746" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="afcae322f938b1831e997e755636afc1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="041f13eb0e079512118c42f2f99b7046" ns3:_="">
     <xsd:import namespace="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
@@ -1102,15 +1002,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A1D3B3-1A39-4D4D-BFE6-D76A5FF26CFE}">
   <ds:schemaRefs>
@@ -1128,6 +1019,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE9D510-3DE7-4BF6-9275-165518CBD85E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB112CA5-772D-401E-B7BD-FCD9C5E40A48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,12 +1042,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE9D510-3DE7-4BF6-9275-165518CBD85E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Goof progress on the irf functionality
</commit_message>
<xml_diff>
--- a/Utilities/prior_table.xlsx
+++ b/Utilities/prior_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoamarante/PycharmProjects/pydsge/Utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gusamarante/PycharmProjects/pydsge/Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF6F41-B5A7-744D-8C89-7A25BF8076B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881B2C21-AD81-0A49-B8E6-16C791BB1671}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19440" windowHeight="15160" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
+    <workbookView xWindow="600" yWindow="840" windowWidth="19440" windowHeight="15160" activeTab="1" xr2:uid="{9C8F70A8-B544-4550-8910-7BBB2082FCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Priors" sheetId="1" r:id="rId1"/>
@@ -282,12 +282,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,6 +298,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6ADE82D-4C65-4E41-9CFD-12B21879D657}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -655,10 +655,10 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>0.5</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="14">
         <v>0.2</v>
       </c>
       <c r="D4" s="3">
@@ -674,10 +674,10 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>0.24800000000000003</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>9.9599196783909855E-2</v>
       </c>
       <c r="D5" s="3">
@@ -693,10 +693,10 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>0.4999999999426315</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>0.250000000005138</v>
       </c>
       <c r="D6" s="3">
@@ -712,10 +712,10 @@
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="15">
         <v>0.5</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>0.28867513459481287</v>
       </c>
       <c r="D7" s="3">
@@ -731,10 +731,10 @@
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>3</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <v>3</v>
       </c>
       <c r="D8" s="3">
@@ -756,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DF6D28-0B61-407D-A00A-C6152F94AC75}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -783,10 +783,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
@@ -808,7 +808,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="12">
-        <v>44023.5</v>
+        <v>44183.916666666664</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
       </c>
       <c r="F9" s="11">
         <f ca="1">(F7-NOW())*24*3600*B11</f>
-        <v>183448.58757089984</v>
+        <v>36633.402000339702</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -839,8 +839,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="4">
-        <f>B6/(B9+60*B8+3600*B7)</f>
-        <v>2.8248587570621471</v>
+        <v>3.4</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -856,21 +855,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D294B0ABAE3DD40AEF644D986102746" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="afcae322f938b1831e997e755636afc1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="041f13eb0e079512118c42f2f99b7046" ns3:_="">
     <xsd:import namespace="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
@@ -1002,31 +986,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A1D3B3-1A39-4D4D-BFE6-D76A5FF26CFE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE9D510-3DE7-4BF6-9275-165518CBD85E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB112CA5-772D-401E-B7BD-FCD9C5E40A48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1042,4 +1017,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE9D510-3DE7-4BF6-9275-165518CBD85E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37A1D3B3-1A39-4D4D-BFE6-D76A5FF26CFE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d22803a6-8dcd-4dbb-9a34-5660fc76e5ef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>